<commit_message>
Chnge to relay board
</commit_message>
<xml_diff>
--- a/RemoteLaunch_Controller/4ChWirelessLaunchController - try 2 w relay pcb/4ch Mouser BOM.xlsx
+++ b/RemoteLaunch_Controller/4ChWirelessLaunchController - try 2 w relay pcb/4ch Mouser BOM.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_A20E88DF0A031667765CAD4540D6300A25D533DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48F179AA-58B1-4ACB-B179-288802C217B3}"/>
   <bookViews>
-    <workbookView xWindow="1270" yWindow="520" windowWidth="17840" windowHeight="8460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="525" windowWidth="17835" windowHeight="8460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="104">
   <si>
     <t xml:space="preserve">Item </t>
   </si>
@@ -51,9 +51,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Tot</t>
-  </si>
-  <si>
     <t>TB007-508-02BE</t>
   </si>
   <si>
@@ -337,13 +334,22 @@
   </si>
   <si>
     <t>70HFR120</t>
+  </si>
+  <si>
+    <t>push button</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07W4LCP1J/ref=ppx_yo_dt_b_asin_image_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>12mm Metal Boat Horn Momentary Push Button Stainless Steel Starter Switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,7 +401,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -408,6 +414,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -682,43 +694,43 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="32.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" customWidth="1"/>
-    <col min="6" max="6" width="23.1796875" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="4"/>
-    <col min="8" max="8" width="18.453125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="67.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="4"/>
+    <col min="8" max="8" width="67.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -726,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
@@ -734,47 +746,40 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
       </c>
       <c r="G4" s="4">
         <v>0.73</v>
       </c>
-      <c r="H4" s="5">
-        <f>G4*C4</f>
-        <v>1.46</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>2</v>
       </c>
@@ -782,26 +787,22 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
         <v>10</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="G5" s="4">
         <v>1.18</v>
       </c>
-      <c r="H5" s="5">
-        <f t="shared" ref="H5:H9" si="0">G5*C5</f>
-        <v>4.72</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>3</v>
       </c>
@@ -809,873 +810,1341 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
+      <c r="F6" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="G6" s="4">
         <v>1.77</v>
       </c>
-      <c r="H6" s="5">
-        <f t="shared" si="0"/>
-        <v>1.77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:9">
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="G7" s="4">
         <v>1.32</v>
       </c>
-      <c r="H7" s="5">
-        <f t="shared" si="0"/>
-        <v>6.6000000000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:9">
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
       </c>
       <c r="G8" s="4">
         <v>0.15</v>
       </c>
-      <c r="H8" s="5">
-        <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:9">
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="4">
         <v>10</v>
       </c>
-      <c r="H9" s="5">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9">
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G10" s="4">
         <v>0.46</v>
       </c>
-      <c r="H10" s="5">
-        <f t="shared" ref="H10" si="1">G10*C10*2</f>
-        <v>3.68</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J11" s="4">
+      <c r="H10" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="I11" s="4">
         <f>SUM(G4:G9)</f>
         <v>15.15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>48</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
       </c>
       <c r="G13" s="5">
         <v>34.950000000000003</v>
       </c>
-      <c r="H13" s="5">
-        <f>G13*C13*2</f>
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:9">
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
         <v>7</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="G14" s="4">
         <v>0.73</v>
       </c>
-      <c r="H14" s="5">
-        <f t="shared" ref="H14:H29" si="2">G14*C14*2</f>
-        <v>2.92</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>19</v>
+      <c r="F15" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="G15" s="4">
         <v>1.77</v>
       </c>
-      <c r="H15" s="5">
-        <f t="shared" si="2"/>
-        <v>7.08</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:9">
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G16" s="4">
         <v>1.72</v>
       </c>
-      <c r="H16" s="5">
-        <f t="shared" si="2"/>
-        <v>6.88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:10">
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s">
         <v>79</v>
       </c>
-      <c r="E17" t="s">
+      <c r="H17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:10">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" t="s">
         <v>82</v>
       </c>
-      <c r="E18" t="s">
-        <v>83</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H18" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
         <v>50</v>
       </c>
-      <c r="E19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19">
+      <c r="F19" s="7">
         <v>2886</v>
       </c>
       <c r="G19" s="4">
         <v>0.95</v>
       </c>
-      <c r="H19" s="5">
-        <f t="shared" si="2"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:10">
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G20" s="4">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H20" s="5">
-        <f t="shared" si="2"/>
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:10">
       <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" t="s">
         <v>57</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="F21" t="s">
-        <v>59</v>
       </c>
       <c r="G21" s="4">
         <v>0.4</v>
       </c>
-      <c r="H21" s="5">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="H21" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" t="s">
         <v>61</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="F22" t="s">
-        <v>63</v>
       </c>
       <c r="G22" s="4">
         <v>0.41</v>
       </c>
-      <c r="H22" s="5">
-        <f t="shared" si="2"/>
-        <v>0.82</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="H22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="B23" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" t="s">
         <v>65</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="F23" t="s">
-        <v>67</v>
       </c>
       <c r="G23" s="4">
         <v>0.44</v>
       </c>
-      <c r="H23" s="5">
-        <f t="shared" si="2"/>
-        <v>0.88</v>
-      </c>
-      <c r="I23" s="2" t="s">
+      <c r="H23" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="F24" t="s">
-        <v>71</v>
       </c>
       <c r="G24" s="4">
         <v>0.6</v>
       </c>
-      <c r="H24" s="5">
-        <f t="shared" si="2"/>
-        <v>1.2</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K24" s="4">
-        <f>SUM(G13:G24)</f>
-        <v>42.55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="H24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="30">
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G25" s="4">
         <v>6.25</v>
       </c>
-      <c r="H25" s="5">
-        <f t="shared" si="2"/>
-        <v>12.5</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H25" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G26" s="4">
         <v>30</v>
       </c>
-      <c r="H26" s="5">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:10">
       <c r="C27">
         <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G27" s="4">
         <v>0.37</v>
       </c>
-      <c r="H27" s="5">
-        <f t="shared" si="2"/>
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:10">
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G28" s="4">
         <v>0.46</v>
       </c>
-      <c r="H28" s="5">
-        <f t="shared" si="2"/>
-        <v>3.68</v>
-      </c>
-      <c r="I28" s="2" t="s">
+      <c r="H28" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="G29" s="4">
         <v>1.4</v>
       </c>
-      <c r="H29" s="5">
-        <f t="shared" si="2"/>
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="J30" s="4">
+    </row>
+    <row r="30" spans="1:10">
+      <c r="I30" s="4">
         <f>SUM(G13:G29)</f>
         <v>81.03</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G32" s="4">
         <v>0.12</v>
       </c>
-      <c r="H32" s="5">
-        <f>G32*C32</f>
-        <v>0.24</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H32" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="45">
       <c r="C33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="4">
+        <v>8</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9">
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9">
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9">
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9">
+      <c r="D37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9">
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" ht="30">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="4">
+        <v>29.99</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" ht="30">
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" s="4">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" ht="30">
+      <c r="D41" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G41" s="4">
+        <v>1</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" ht="30">
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G42" s="4">
+        <v>3</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9">
+      <c r="I48" s="4">
+        <f>SUM(G32:G42)</f>
+        <v>70.11</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9">
+      <c r="I50" s="4"/>
+    </row>
+    <row r="62" spans="9:9">
+      <c r="I62">
+        <f>SUM(I12:I61)</f>
+        <v>151.13999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E24" r:id="rId1" display="https://www.mouser.com/ProductDetail/Kingbright/APA2107LSECK-J4-PRV?qs=6oMev5NRZMFINHnQutSYHA%3D%3D"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="4"/>
+    <col min="8" max="8" width="67.28515625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1.18</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.46</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="I11" s="4">
+        <f>SUM(G4:G9)</f>
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="5">
+        <v>34.950000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2886</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="30">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="4">
+        <v>6.25</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0.46</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="I30" s="4">
+        <f>SUM(G13:G29)</f>
+        <v>81.03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E33" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="4">
         <v>3.88</v>
       </c>
-      <c r="H33" s="5">
-        <f t="shared" ref="H33:H58" si="3">G33*C33</f>
-        <v>7.76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:9">
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G34" s="4">
         <v>3.5</v>
       </c>
-      <c r="H34" s="5">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="H34" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="45">
       <c r="C35">
         <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G35" s="4">
         <v>2</v>
       </c>
-      <c r="H35" s="5">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="I35" s="2" t="s">
+      <c r="H35" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" t="s">
-        <v>87</v>
       </c>
       <c r="G36" s="4">
         <v>3</v>
       </c>
-      <c r="H36" s="5">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:9">
       <c r="C37">
         <v>4</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G37" s="4">
         <v>0.5</v>
       </c>
-      <c r="H37" s="5">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H37" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G38" s="4">
         <v>1.25</v>
       </c>
-      <c r="H38" s="5">
-        <f t="shared" si="3"/>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:9" ht="30">
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G39" s="4">
         <v>29.99</v>
       </c>
-      <c r="H39" s="5">
-        <f t="shared" si="3"/>
-        <v>29.99</v>
-      </c>
-      <c r="I39" s="2" t="s">
+      <c r="H39" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2" t="s">
+    <row r="41" spans="1:9">
+      <c r="D41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H40" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:9">
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H42" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30">
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G43" s="5">
         <v>1.25</v>
       </c>
-      <c r="H43" s="5">
-        <f t="shared" si="3"/>
-        <v>1.25</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="H43" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30">
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G44" s="4">
         <v>0.5</v>
       </c>
-      <c r="H44" s="5">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H44" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45">
       <c r="D45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J46" s="4">
-        <f>SUM(H32:H45)</f>
-        <v>62.489999999999995</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:9">
+      <c r="I46" s="4" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G48" s="4">
         <v>0.12</v>
       </c>
-      <c r="H48" s="5">
-        <f t="shared" si="3"/>
-        <v>0.12</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="H48" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8">
       <c r="C49">
         <v>2</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G49" s="4">
         <v>3.5</v>
       </c>
-      <c r="H49" s="5">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="3:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="H49" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" ht="45">
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G50" s="4">
         <v>2</v>
       </c>
-      <c r="H50" s="5">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="3:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H50" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" ht="45">
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G52" s="4">
         <v>5.75</v>
       </c>
-      <c r="H52" s="5">
-        <f t="shared" si="3"/>
-        <v>5.75</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="H52" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8">
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G53" s="4">
         <v>1.25</v>
       </c>
-      <c r="H53" s="5">
-        <f t="shared" si="3"/>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="54" spans="3:9" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="3:8" ht="30">
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G54" s="4">
         <v>29.99</v>
       </c>
-      <c r="H54" s="5">
-        <f t="shared" si="3"/>
-        <v>29.99</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="3:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H54" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" ht="45">
       <c r="C55">
         <v>5</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G55" s="4">
         <v>3.75</v>
       </c>
-      <c r="H55" s="5">
-        <f t="shared" si="3"/>
-        <v>18.75</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="H55" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8">
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H56" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8">
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G57" s="4">
         <v>0.5</v>
       </c>
-      <c r="H57" s="5">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="58" spans="3:9" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="3:8" ht="45">
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G58" s="4">
         <v>3</v>
       </c>
-      <c r="H58" s="5">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H67" s="5">
-        <f>SUM(H1:H61)</f>
-        <v>336.05</v>
+      <c r="H58" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E24" r:id="rId1" display="https://www.mouser.com/ProductDetail/Kingbright/APA2107LSECK-J4-PRV?qs=6oMev5NRZMFINHnQutSYHA%3D%3D" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E33" r:id="rId2" display="https://www.mouser.com/ProductDetail/665-AI-4228-TWT-R" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E24" r:id="rId1" display="https://www.mouser.com/ProductDetail/Kingbright/APA2107LSECK-J4-PRV?qs=6oMev5NRZMFINHnQutSYHA%3D%3D"/>
+    <hyperlink ref="E33" r:id="rId2" display="https://www.mouser.com/ProductDetail/665-AI-4228-TWT-R"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>